<commit_message>
Menyamakan tabel dengan di laporan
</commit_message>
<xml_diff>
--- a/database/seeders/data_barang.xlsx
+++ b/database/seeders/data_barang.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\inventory_eoq\database\seeders\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9617E1F-75F3-4433-BA12-13238FC325DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B83EEA20-1AD0-4E4F-BC84-D4058D115489}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{164D28EB-19A2-46B5-9A43-4782667B0A5D}"/>
+    <workbookView xWindow="5400" yWindow="3996" windowWidth="13200" windowHeight="8964" xr2:uid="{164D28EB-19A2-46B5-9A43-4782667B0A5D}"/>
   </bookViews>
   <sheets>
-    <sheet name="barangs" sheetId="1" r:id="rId1"/>
+    <sheet name="barang" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -433,7 +433,7 @@
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -470,7 +470,7 @@
       </c>
       <c r="D2">
         <f ca="1">RANDBETWEEN(30,60)</f>
-        <v>35</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
@@ -485,7 +485,7 @@
       </c>
       <c r="D3">
         <f t="shared" ref="D3:D9" ca="1" si="0">RANDBETWEEN(30,60)</f>
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
@@ -500,7 +500,7 @@
       </c>
       <c r="D4">
         <f t="shared" ca="1" si="0"/>
-        <v>49</v>
+        <v>57</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
@@ -515,7 +515,7 @@
       </c>
       <c r="D5">
         <f t="shared" ca="1" si="0"/>
-        <v>34</v>
+        <v>45</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
@@ -530,7 +530,7 @@
       </c>
       <c r="D6">
         <f t="shared" ca="1" si="0"/>
-        <v>51</v>
+        <v>54</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
@@ -545,7 +545,7 @@
       </c>
       <c r="D7">
         <f t="shared" ca="1" si="0"/>
-        <v>36</v>
+        <v>60</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
@@ -560,7 +560,7 @@
       </c>
       <c r="D8">
         <f t="shared" ca="1" si="0"/>
-        <v>46</v>
+        <v>60</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
@@ -575,7 +575,7 @@
       </c>
       <c r="D9">
         <f t="shared" ca="1" si="0"/>
-        <v>58</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>